<commit_message>
cambio de direccion HEX to BIN
</commit_message>
<xml_diff>
--- a/protocolos_status.xlsx
+++ b/protocolos_status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="239">
   <si>
     <t>Aprobado</t>
   </si>
@@ -724,6 +724,15 @@
   </si>
   <si>
     <t>OTP CHECK SUM</t>
+  </si>
+  <si>
+    <t>FC1FH</t>
+  </si>
+  <si>
+    <t>F6B3H</t>
+  </si>
+  <si>
+    <t>F661H</t>
   </si>
 </sst>
 </file>
@@ -1008,14 +1017,14 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1323,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="D97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1395,6 +1404,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="6"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
@@ -1416,6 +1426,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="6"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
@@ -1439,7 +1450,7 @@
       <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="22" t="s">
         <v>234</v>
       </c>
     </row>
@@ -1463,6 +1474,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="6"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
@@ -1484,6 +1496,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="6"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
@@ -1505,6 +1518,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="6"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
@@ -1526,6 +1540,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="6"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
@@ -1549,7 +1564,7 @@
       <c r="G10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="22" t="s">
         <v>233</v>
       </c>
     </row>
@@ -1573,6 +1588,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="4"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
@@ -1594,6 +1610,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="4"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
@@ -1615,6 +1632,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="4"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
@@ -1636,6 +1654,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="4"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
@@ -1657,6 +1676,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="7"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="15" t="s">
@@ -1678,8 +1698,9 @@
         <v>3</v>
       </c>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="16"/>
       <c r="B17" s="5" t="s">
         <v>72</v>
@@ -1695,8 +1716,9 @@
         <v>3</v>
       </c>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="16"/>
       <c r="B18" s="5" t="s">
         <v>73</v>
@@ -1712,8 +1734,9 @@
         <v>3</v>
       </c>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="16"/>
       <c r="B19" s="5" t="s">
         <v>75</v>
@@ -1729,8 +1752,9 @@
         <v>3</v>
       </c>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="16"/>
       <c r="B20" s="5" t="s">
         <v>77</v>
@@ -1746,8 +1770,9 @@
         <v>3</v>
       </c>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="16"/>
       <c r="B21" s="5" t="s">
         <v>78</v>
@@ -1763,8 +1788,9 @@
         <v>3</v>
       </c>
       <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="16"/>
       <c r="B22" s="5" t="s">
         <v>80</v>
@@ -1780,8 +1806,9 @@
         <v>3</v>
       </c>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="16"/>
       <c r="B23" s="5" t="s">
         <v>81</v>
@@ -1797,8 +1824,9 @@
         <v>3</v>
       </c>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="16"/>
       <c r="B24" s="5" t="s">
         <v>83</v>
@@ -1814,8 +1842,9 @@
         <v>3</v>
       </c>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="5" t="s">
         <v>85</v>
@@ -1831,8 +1860,9 @@
         <v>3</v>
       </c>
       <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="16"/>
       <c r="B26" s="5" t="s">
         <v>87</v>
@@ -1848,8 +1878,9 @@
         <v>3</v>
       </c>
       <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="16"/>
       <c r="B27" s="5" t="s">
         <v>89</v>
@@ -1865,8 +1896,9 @@
         <v>3</v>
       </c>
       <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="16"/>
       <c r="B28" s="5" t="s">
         <v>90</v>
@@ -1882,8 +1914,9 @@
         <v>3</v>
       </c>
       <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="16"/>
       <c r="B29" s="5" t="s">
         <v>91</v>
@@ -1899,8 +1932,9 @@
         <v>3</v>
       </c>
       <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="21"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="16"/>
       <c r="B30" s="5" t="s">
         <v>92</v>
@@ -1916,8 +1950,9 @@
         <v>3</v>
       </c>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="16"/>
       <c r="B31" s="5" t="s">
         <v>93</v>
@@ -1933,8 +1968,9 @@
         <v>3</v>
       </c>
       <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="21"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="16"/>
       <c r="B32" s="5" t="s">
         <v>95</v>
@@ -1950,8 +1986,9 @@
         <v>3</v>
       </c>
       <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="16"/>
       <c r="B33" s="5" t="s">
         <v>97</v>
@@ -1967,8 +2004,9 @@
         <v>3</v>
       </c>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="16"/>
       <c r="B34" s="5" t="s">
         <v>99</v>
@@ -1984,8 +2022,9 @@
         <v>3</v>
       </c>
       <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="16"/>
       <c r="B35" s="5" t="s">
         <v>101</v>
@@ -2001,8 +2040,9 @@
         <v>3</v>
       </c>
       <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="16"/>
       <c r="B36" s="5" t="s">
         <v>103</v>
@@ -2018,8 +2058,9 @@
         <v>3</v>
       </c>
       <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="16"/>
       <c r="B37" s="5" t="s">
         <v>105</v>
@@ -2035,8 +2076,9 @@
         <v>3</v>
       </c>
       <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="16"/>
       <c r="B38" s="5" t="s">
         <v>107</v>
@@ -2052,8 +2094,9 @@
         <v>3</v>
       </c>
       <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="16"/>
       <c r="B39" s="5" t="s">
         <v>108</v>
@@ -2069,8 +2112,9 @@
         <v>3</v>
       </c>
       <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="16"/>
       <c r="B40" s="5" t="s">
         <v>110</v>
@@ -2086,8 +2130,9 @@
         <v>3</v>
       </c>
       <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="21"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="16"/>
       <c r="B41" s="5" t="s">
         <v>112</v>
@@ -2103,8 +2148,9 @@
         <v>3</v>
       </c>
       <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="21"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="16"/>
       <c r="B42" s="5" t="s">
         <v>113</v>
@@ -2120,8 +2166,9 @@
         <v>3</v>
       </c>
       <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="21"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="16"/>
       <c r="B43" s="5" t="s">
         <v>115</v>
@@ -2137,8 +2184,9 @@
         <v>3</v>
       </c>
       <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" s="21"/>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="16"/>
       <c r="B44" s="5" t="s">
         <v>117</v>
@@ -2154,8 +2202,9 @@
         <v>3</v>
       </c>
       <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44" s="21"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="16"/>
       <c r="B45" s="5" t="s">
         <v>119</v>
@@ -2171,8 +2220,9 @@
         <v>3</v>
       </c>
       <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" s="21"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="16"/>
       <c r="B46" s="5" t="s">
         <v>120</v>
@@ -2188,8 +2238,9 @@
         <v>3</v>
       </c>
       <c r="G46" s="4"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="16"/>
       <c r="B47" s="5" t="s">
         <v>122</v>
@@ -2205,8 +2256,9 @@
         <v>3</v>
       </c>
       <c r="G47" s="4"/>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="16"/>
       <c r="B48" s="5" t="s">
         <v>123</v>
@@ -2222,8 +2274,9 @@
         <v>3</v>
       </c>
       <c r="G48" s="4"/>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" s="21"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="16"/>
       <c r="B49" s="5" t="s">
         <v>125</v>
@@ -2239,8 +2292,9 @@
         <v>3</v>
       </c>
       <c r="G49" s="4"/>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="16"/>
       <c r="B50" s="5" t="s">
         <v>127</v>
@@ -2256,8 +2310,9 @@
         <v>3</v>
       </c>
       <c r="G50" s="4"/>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="21"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="16"/>
       <c r="B51" s="5" t="s">
         <v>129</v>
@@ -2273,8 +2328,9 @@
         <v>3</v>
       </c>
       <c r="G51" s="4"/>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="21"/>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="16"/>
       <c r="B52" s="5" t="s">
         <v>131</v>
@@ -2290,8 +2346,9 @@
         <v>3</v>
       </c>
       <c r="G52" s="4"/>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="21"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="5" t="s">
         <v>132</v>
@@ -2307,8 +2364,9 @@
         <v>3</v>
       </c>
       <c r="G53" s="4"/>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="15" t="s">
         <v>134</v>
       </c>
@@ -2328,8 +2386,9 @@
         <v>3</v>
       </c>
       <c r="G54" s="4"/>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" s="21"/>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="16"/>
       <c r="B55" s="5" t="s">
         <v>137</v>
@@ -2345,8 +2404,9 @@
         <v>3</v>
       </c>
       <c r="G55" s="4"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="21"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="16"/>
       <c r="B56" s="5" t="s">
         <v>138</v>
@@ -2362,8 +2422,9 @@
         <v>3</v>
       </c>
       <c r="G56" s="4"/>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="21"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="16"/>
       <c r="B57" s="5" t="s">
         <v>139</v>
@@ -2379,8 +2440,9 @@
         <v>3</v>
       </c>
       <c r="G57" s="4"/>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="21"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="16"/>
       <c r="B58" s="5" t="s">
         <v>140</v>
@@ -2396,8 +2458,9 @@
         <v>3</v>
       </c>
       <c r="G58" s="4"/>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="16"/>
       <c r="B59" s="5" t="s">
         <v>141</v>
@@ -2413,8 +2476,9 @@
         <v>3</v>
       </c>
       <c r="G59" s="4"/>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="21"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="16"/>
       <c r="B60" s="5" t="s">
         <v>142</v>
@@ -2430,8 +2494,9 @@
         <v>3</v>
       </c>
       <c r="G60" s="4"/>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="16"/>
       <c r="B61" s="5" t="s">
         <v>144</v>
@@ -2447,8 +2512,9 @@
         <v>3</v>
       </c>
       <c r="G61" s="4"/>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="21"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="16"/>
       <c r="B62" s="5" t="s">
         <v>145</v>
@@ -2464,8 +2530,9 @@
         <v>3</v>
       </c>
       <c r="G62" s="4"/>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="21"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="16"/>
       <c r="B63" s="5" t="s">
         <v>146</v>
@@ -2481,8 +2548,9 @@
         <v>3</v>
       </c>
       <c r="G63" s="4"/>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="21"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="16"/>
       <c r="B64" s="5" t="s">
         <v>147</v>
@@ -2498,8 +2566,9 @@
         <v>3</v>
       </c>
       <c r="G64" s="4"/>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="21"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="16"/>
       <c r="B65" s="5" t="s">
         <v>148</v>
@@ -2515,8 +2584,9 @@
         <v>3</v>
       </c>
       <c r="G65" s="4"/>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" s="21"/>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="16"/>
       <c r="B66" s="5" t="s">
         <v>149</v>
@@ -2532,8 +2602,9 @@
         <v>3</v>
       </c>
       <c r="G66" s="4"/>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" s="21"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="16"/>
       <c r="B67" s="5" t="s">
         <v>150</v>
@@ -2549,8 +2620,9 @@
         <v>3</v>
       </c>
       <c r="G67" s="4"/>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" s="21"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="16"/>
       <c r="B68" s="5" t="s">
         <v>151</v>
@@ -2566,8 +2638,9 @@
         <v>3</v>
       </c>
       <c r="G68" s="4"/>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" s="21"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="16"/>
       <c r="B69" s="5" t="s">
         <v>152</v>
@@ -2583,8 +2656,9 @@
         <v>3</v>
       </c>
       <c r="G69" s="4"/>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" s="21"/>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="16"/>
       <c r="B70" s="5" t="s">
         <v>153</v>
@@ -2600,8 +2674,9 @@
         <v>3</v>
       </c>
       <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="H70" s="21"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="16"/>
       <c r="B71" s="5" t="s">
         <v>154</v>
@@ -2617,8 +2692,9 @@
         <v>3</v>
       </c>
       <c r="G71" s="4"/>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" s="21"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="16"/>
       <c r="B72" s="5" t="s">
         <v>155</v>
@@ -2634,8 +2710,9 @@
         <v>3</v>
       </c>
       <c r="G72" s="4"/>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="H72" s="21"/>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="16"/>
       <c r="B73" s="5" t="s">
         <v>156</v>
@@ -2651,8 +2728,9 @@
         <v>3</v>
       </c>
       <c r="G73" s="4"/>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" s="21"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="16"/>
       <c r="B74" s="5" t="s">
         <v>157</v>
@@ -2668,8 +2746,9 @@
         <v>3</v>
       </c>
       <c r="G74" s="4"/>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" s="21"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="16"/>
       <c r="B75" s="5" t="s">
         <v>158</v>
@@ -2685,8 +2764,9 @@
         <v>3</v>
       </c>
       <c r="G75" s="4"/>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" s="21"/>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="16"/>
       <c r="B76" s="5" t="s">
         <v>159</v>
@@ -2702,8 +2782,9 @@
         <v>3</v>
       </c>
       <c r="G76" s="4"/>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" s="21"/>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="16"/>
       <c r="B77" s="5" t="s">
         <v>160</v>
@@ -2719,8 +2800,9 @@
         <v>3</v>
       </c>
       <c r="G77" s="4"/>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77" s="21"/>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="16"/>
       <c r="B78" s="5" t="s">
         <v>161</v>
@@ -2736,8 +2818,9 @@
         <v>3</v>
       </c>
       <c r="G78" s="4"/>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" s="21"/>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="16"/>
       <c r="B79" s="5" t="s">
         <v>162</v>
@@ -2753,8 +2836,9 @@
         <v>3</v>
       </c>
       <c r="G79" s="4"/>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="H79" s="21"/>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="16"/>
       <c r="B80" s="5" t="s">
         <v>163</v>
@@ -2770,8 +2854,9 @@
         <v>3</v>
       </c>
       <c r="G80" s="4"/>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80" s="21"/>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="16"/>
       <c r="B81" s="5" t="s">
         <v>164</v>
@@ -2787,8 +2872,9 @@
         <v>3</v>
       </c>
       <c r="G81" s="4"/>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" s="21"/>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="16"/>
       <c r="B82" s="5" t="s">
         <v>165</v>
@@ -2804,8 +2890,9 @@
         <v>3</v>
       </c>
       <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82" s="21"/>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="16"/>
       <c r="B83" s="5" t="s">
         <v>166</v>
@@ -2821,8 +2908,9 @@
         <v>3</v>
       </c>
       <c r="G83" s="4"/>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83" s="21"/>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="16"/>
       <c r="B84" s="5" t="s">
         <v>167</v>
@@ -2838,8 +2926,9 @@
         <v>3</v>
       </c>
       <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="H84" s="21"/>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="16"/>
       <c r="B85" s="5" t="s">
         <v>168</v>
@@ -2855,8 +2944,9 @@
         <v>3</v>
       </c>
       <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85" s="21"/>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="16"/>
       <c r="B86" s="5" t="s">
         <v>169</v>
@@ -2872,8 +2962,9 @@
         <v>3</v>
       </c>
       <c r="G86" s="4"/>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="H86" s="21"/>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="16"/>
       <c r="B87" s="5" t="s">
         <v>170</v>
@@ -2889,8 +2980,9 @@
         <v>3</v>
       </c>
       <c r="G87" s="4"/>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="H87" s="21"/>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="16"/>
       <c r="B88" s="5" t="s">
         <v>171</v>
@@ -2906,8 +2998,9 @@
         <v>3</v>
       </c>
       <c r="G88" s="4"/>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="H88" s="21"/>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" s="16"/>
       <c r="B89" s="5" t="s">
         <v>172</v>
@@ -2923,8 +3016,9 @@
         <v>3</v>
       </c>
       <c r="G89" s="4"/>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" s="21"/>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="16"/>
       <c r="B90" s="5" t="s">
         <v>173</v>
@@ -2940,8 +3034,9 @@
         <v>3</v>
       </c>
       <c r="G90" s="4"/>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" s="21"/>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="16"/>
       <c r="B91" s="5" t="s">
         <v>174</v>
@@ -2957,8 +3052,9 @@
         <v>3</v>
       </c>
       <c r="G91" s="4"/>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="H91" s="21"/>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="16"/>
       <c r="B92" s="5" t="s">
         <v>175</v>
@@ -2974,8 +3070,9 @@
         <v>3</v>
       </c>
       <c r="G92" s="4"/>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="H92" s="21"/>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="16"/>
       <c r="B93" s="5" t="s">
         <v>176</v>
@@ -2991,8 +3088,9 @@
         <v>3</v>
       </c>
       <c r="G93" s="4"/>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93" s="21"/>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="5" t="s">
         <v>177</v>
@@ -3008,8 +3106,9 @@
         <v>3</v>
       </c>
       <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" s="21"/>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="3" t="s">
         <v>179</v>
       </c>
@@ -3029,8 +3128,9 @@
         <v>3</v>
       </c>
       <c r="G95" s="4"/>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="H95" s="21"/>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="3" t="s">
         <v>182</v>
       </c>
@@ -3050,8 +3150,9 @@
         <v>3</v>
       </c>
       <c r="G96" s="4"/>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="H96" s="21"/>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="3" t="s">
         <v>185</v>
       </c>
@@ -3071,8 +3172,9 @@
         <v>3</v>
       </c>
       <c r="G97" s="4"/>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="H97" s="21"/>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="3" t="s">
         <v>188</v>
       </c>
@@ -3092,8 +3194,9 @@
         <v>3</v>
       </c>
       <c r="G98" s="4"/>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="H98" s="21"/>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="3" t="s">
         <v>191</v>
       </c>
@@ -3113,15 +3216,16 @@
         <v>3</v>
       </c>
       <c r="G99" s="4"/>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="26" t="s">
+      <c r="H99" s="21"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="27" t="s">
         <v>195</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C100" s="25" t="s">
+      <c r="C100" s="26" t="s">
         <v>197</v>
       </c>
       <c r="D100" s="6" t="s">
@@ -3134,13 +3238,16 @@
         <v>3</v>
       </c>
       <c r="G100" s="4"/>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="26"/>
+      <c r="H100" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="27"/>
       <c r="B101" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C101" s="25"/>
+      <c r="C101" s="26"/>
       <c r="D101" s="6" t="s">
         <v>200</v>
       </c>
@@ -3151,32 +3258,38 @@
         <v>3</v>
       </c>
       <c r="G101" s="4"/>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="26"/>
+      <c r="H101" s="22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="27"/>
       <c r="B102" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="25"/>
+      <c r="C102" s="26"/>
       <c r="D102" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E102" s="27" t="s">
+      <c r="E102" s="25" t="s">
         <v>1</v>
       </c>
       <c r="F102" s="20" t="s">
         <v>3</v>
       </c>
       <c r="G102" s="4"/>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="H102" s="22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C103" s="25" t="s">
+      <c r="C103" s="26" t="s">
         <v>204</v>
       </c>
       <c r="D103" s="6" t="s">
@@ -3189,15 +3302,16 @@
         <v>3</v>
       </c>
       <c r="G103" s="4"/>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="H103" s="21"/>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C104" s="25"/>
+      <c r="C104" s="26"/>
       <c r="D104" s="6" t="s">
         <v>20</v>
       </c>
@@ -3208,8 +3322,9 @@
         <v>3</v>
       </c>
       <c r="G104" s="4"/>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="H104" s="21"/>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="3" t="s">
         <v>206</v>
       </c>
@@ -3229,8 +3344,9 @@
         <v>3</v>
       </c>
       <c r="G105" s="4"/>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="H105" s="21"/>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" s="3" t="s">
         <v>209</v>
       </c>
@@ -3250,8 +3366,9 @@
         <v>3</v>
       </c>
       <c r="G106" s="4"/>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" s="21"/>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" s="3" t="s">
         <v>212</v>
       </c>
@@ -3271,8 +3388,9 @@
         <v>3</v>
       </c>
       <c r="G107" s="4"/>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" s="21"/>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" s="3" t="s">
         <v>216</v>
       </c>
@@ -3292,8 +3410,9 @@
         <v>3</v>
       </c>
       <c r="G108" s="4"/>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="H108" s="21"/>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" s="3" t="s">
         <v>220</v>
       </c>
@@ -3313,8 +3432,9 @@
         <v>3</v>
       </c>
       <c r="G109" s="4"/>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="H109" s="21"/>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" s="3" t="s">
         <v>224</v>
       </c>
@@ -3334,8 +3454,9 @@
         <v>3</v>
       </c>
       <c r="G110" s="4"/>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="H110" s="21"/>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" s="3" t="s">
         <v>228</v>
       </c>
@@ -3355,6 +3476,7 @@
         <v>3</v>
       </c>
       <c r="G111" s="4"/>
+      <c r="H111" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>